<commit_message>
[ENH] Added following funcitonalities: test and noise variable time defined in config, noise among trials, down button for unknown answer, code reorganization
</commit_message>
<xml_diff>
--- a/src/begiBrainDemo/colors_to_test.xlsx
+++ b/src/begiBrainDemo/colors_to_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akoun\Desktop\Biocruces\siburmuin\src\begiBrainDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{980B1596-DAAD-47C0-9005-D12027E8040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CF54B0-14EB-47CE-8FC4-712EB6C9684D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{E5458DB3-6A1D-4BE3-8E91-52D53E0F1609}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{E5458DB3-6A1D-4BE3-8E91-52D53E0F1609}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>color_h</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>test_color</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -504,11 +516,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.73046875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -516,7 +528,7 @@
     <col min="1" max="1" width="20.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -526,19 +538,25 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -547,6 +565,23 @@
       </c>
       <c r="C3">
         <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -562,6 +597,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -675,22 +725,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -704,27 +762,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[ENH] Added multiple saturation ranges to test in color staircase test
</commit_message>
<xml_diff>
--- a/src/begiBrainDemo/colors_to_test.xlsx
+++ b/src/begiBrainDemo/colors_to_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akoun\Desktop\Biocruces\siburmuin\src\begiBrainDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CF54B0-14EB-47CE-8FC4-712EB6C9684D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774649E1-1B24-45F5-819D-C451BE1A2541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{E5458DB3-6A1D-4BE3-8E91-52D53E0F1609}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{E5458DB3-6A1D-4BE3-8E91-52D53E0F1609}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>color_h</t>
   </si>
@@ -116,13 +116,16 @@
     <t>test_color</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>low</t>
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>color_saturation_type</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -539,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -553,35 +556,63 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>180</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>100</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>